<commit_message>
Stage 6. A check for uniqueness is added. The error page was changed.
</commit_message>
<xml_diff>
--- a/GroupSplin.xlsx
+++ b/GroupSplin.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="18">
   <si>
     <t>Alexander Vasiliev</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>Birdzina Murgulia</t>
+  </si>
+  <si>
+    <t>Birdzina Muкia</t>
+  </si>
+  <si>
+    <t>авва</t>
   </si>
 </sst>
 </file>
@@ -399,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -414,6 +420,7 @@
     <col min="5" max="5" width="10.33203125" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" customWidth="1"/>
     <col min="7" max="7" width="11.44140625" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -467,21 +474,67 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1">
         <v>25399</v>
       </c>
       <c r="D3">
-        <v>1234567891</v>
+        <v>7345934509</v>
       </c>
       <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>21746</v>
+      </c>
+      <c r="D4">
+        <v>7345934509</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>25399</v>
+      </c>
+      <c r="D5">
+        <v>7345934509</v>
+      </c>
+      <c r="E5" t="s">
         <v>11</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F5" t="s">
         <v>12</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G5" t="s">
         <v>13</v>
       </c>
     </row>
@@ -492,10 +545,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -574,6 +627,29 @@
         <v>13</v>
       </c>
     </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1">
+        <v>29906</v>
+      </c>
+      <c r="D4">
+        <v>6756453423</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>